<commit_message>
debugging the input data process
</commit_message>
<xml_diff>
--- a/data/energy_data.xlsx
+++ b/data/energy_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saeed.misaghian\Documents\Training\Udacity_ML_Engineering\Final_projecrt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saeed.misaghian\Documents\Repos_Personal\Azure_ML_Energy_Predict\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CEA885-5121-4C29-9FC3-771D7F14E5B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF51ED8-D76B-4E97-96F9-BFA02988CC43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="17232" windowHeight="6216" tabRatio="594" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10500" tabRatio="594" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>

</xml_diff>